<commit_message>
fix about page typos
</commit_message>
<xml_diff>
--- a/src/data/COPD COMPAR-EU Data.xlsx
+++ b/src/data/COPD COMPAR-EU Data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Εxacerbations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Exacerbations" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="EmergencyRoom_COPD" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Emergency_room_Allcause" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Emergency_room_Allcause!$A$1:$I$38</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">EmergencyRoom_COPD!$A$1:$I$38</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Εxacerbations!$A$1:$D$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Exacerbations!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -349,11 +349,11 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.16"/>
@@ -803,7 +803,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.16"/>
@@ -1431,11 +1431,11 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.16"/>

</xml_diff>